<commit_message>
增加Connect SIM Card List部分接口用例
</commit_message>
<xml_diff>
--- a/data/connect_cases.xlsx
+++ b/data/connect_cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="1" state="visible" r:id="rId1"/>
@@ -69,6 +69,7 @@
     <font>
       <name val="宋体"/>
       <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
       <scheme val="minor"/>
     </font>
@@ -559,8 +560,8 @@
     <col customWidth="1" max="8" min="8" style="10" width="18.75"/>
     <col customWidth="1" max="9" min="9" style="3" width="19.875"/>
     <col customWidth="1" max="10" min="10" style="10" width="9"/>
-    <col customWidth="1" max="82" min="11" style="3" width="9"/>
-    <col customWidth="1" max="16384" min="83" style="3" width="9"/>
+    <col customWidth="1" max="86" min="11" style="3" width="9"/>
+    <col customWidth="1" max="16384" min="87" style="3" width="9"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="22.5" r="1">
@@ -883,10 +884,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="A3" sqref="A3:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -901,8 +902,8 @@
     <col customWidth="1" max="8" min="8" style="10" width="18.75"/>
     <col customWidth="1" max="9" min="9" style="3" width="19.875"/>
     <col customWidth="1" max="10" min="10" style="10" width="9"/>
-    <col customWidth="1" max="82" min="11" style="3" width="9"/>
-    <col customWidth="1" max="16384" min="83" style="3" width="9"/>
+    <col customWidth="1" max="86" min="11" style="3" width="9"/>
+    <col customWidth="1" max="16384" min="87" style="3" width="9"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="22.5" r="1">
@@ -957,7 +958,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="267" r="2">
+    <row customHeight="1" ht="228.75" r="2">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
@@ -997,6 +998,385 @@
       </c>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="90" r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>添加组--成功</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCardGroup/add</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>{"name":"AutoGR","description":"456"}</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":{"id":"c37fad61fed87eac","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-30T08:27:10Z","updator":"788135736837423104","updateTime":"2022-12-30T08:27:10Z"}}</t>
+        </is>
+      </c>
+      <c r="H3" s="7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>SELECT * FROM `tm_admin`.`simcard_group` WHERE id = '{sim_group_id}';</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="175.5" r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>获取SIM Card Group</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCardGroup/list</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>{"companyId": "{company_id}", 
+"keyword": ""}</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>get</t>
+        </is>
+      </c>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":[{"id":"c37fad61fed87eac","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-30T08:27:10Z","updator":"788135736837423104","updateTime":"2022-12-30T08:27:10Z"}]}</t>
+        </is>
+      </c>
+      <c r="H4" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="n"/>
+      <c r="J4" s="15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="217.5" r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>查询SIM Card List--查询所有SIM Card</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCard/page</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>{
+ "companyId": "{company_id}"
+}</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>get</t>
+        </is>
+      </c>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":{"total":6,"pages":1,"pageSize":10,"pageNum":1,"list":[{"id":"b1fb11141bda5c33","iccid":"8935711220000105110","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528230","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-12-30T08:22:28Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"240af25e16bc2d6a","iccid":"8935711220000105111","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528231","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-11-18T08:24:36Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"c886869e774076aa","iccid":"89430301722233292984","eid":null,"sn":null,"uploadedSn":null,"imsi":"232031723329298","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"d53fc9bf0c152c40","iccid":"89430301722233293008","eid":null,"sn":null,"uploadedSn":null,"imsi":"232031723329300","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"172dc2b31f5532e4","iccid":"89430301722233293180","eid":null,"sn":"TMX0820221029002","uploadedSn":"TMX0820221029002","imsi":"232031723329318","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"c6811af2822eda19","iccid":"89430301722233293198","eid":null,"sn":"TMX0820221029003","uploadedSn":"TMX0820221029003","imsi":"232031723329319","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0}]}}</t>
+        </is>
+      </c>
+      <c r="H5" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I5" s="8" t="n"/>
+      <c r="J5" s="15" t="n"/>
+    </row>
+    <row customHeight="1" ht="175.5" r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>修改SIM Card所属Group</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCard/{first_sim_iccid}/changeGroup?simCardGroupId={sim_group_id}</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>put</t>
+        </is>
+      </c>
+      <c r="F6" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":null}</t>
+        </is>
+      </c>
+      <c r="H6" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I6" s="8" t="n"/>
+      <c r="J6" s="15" t="n"/>
+    </row>
+    <row customHeight="1" ht="175.5" r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>查询SIM Card List--关键字查询</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCard/page</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>{
+ "companyId": "{company_id}",
+ "keyword": "{first_sim_iccid}"
+}</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>get</t>
+        </is>
+      </c>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":{"total":1,"pages":1,"pageSize":10,"pageNum":1,"list":[{"id":"b1fb11141bda5c33","iccid":"8935711220000105110","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528230","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-12-30T08:27:11Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":"c37fad61fed87eac","name":"AutoGR"},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0}]}}</t>
+        </is>
+      </c>
+      <c r="H7" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I7" s="8" t="n"/>
+      <c r="J7" s="15" t="n"/>
+    </row>
+    <row customHeight="1" ht="175.5" r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>查询SIM Card List--根据运营商查询</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCard/page</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>{
+ "companyId": "{company_id}",
+ "providerId": "{carrier_id}"
+}</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>get</t>
+        </is>
+      </c>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":{"total":2,"pages":1,"pageSize":10,"pageNum":1,"list":[{"id":"b1fb11141bda5c33","iccid":"8935711220000105110","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528230","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-12-30T08:27:11Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":"c37fad61fed87eac","name":"AutoGR"},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"240af25e16bc2d6a","iccid":"8935711220000105111","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528231","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-11-18T08:24:36Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0}]}}</t>
+        </is>
+      </c>
+      <c r="H8" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I8" s="8" t="n"/>
+      <c r="J8" s="15" t="n"/>
+    </row>
+    <row customHeight="1" ht="213" r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>查询SIM Card List--根据Status查询</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCard/page</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>{
+ "companyId": "{company_id}",
+ "localSimStatus": "Activated"
+}</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>get</t>
+        </is>
+      </c>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":{"total":6,"pages":1,"pageSize":10,"pageNum":1,"list":[{"id":"b1fb11141bda5c33","iccid":"8935711220000105110","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528230","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-12-30T08:27:11Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":"c37fad61fed87eac","name":"AutoGR"},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"240af25e16bc2d6a","iccid":"8935711220000105111","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528231","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-11-18T08:24:36Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"c886869e774076aa","iccid":"89430301722233292984","eid":null,"sn":null,"uploadedSn":null,"imsi":"232031723329298","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"d53fc9bf0c152c40","iccid":"89430301722233293008","eid":null,"sn":null,"uploadedSn":null,"imsi":"232031723329300","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"172dc2b31f5532e4","iccid":"89430301722233293180","eid":null,"sn":"TMX0820221029002","uploadedSn":"TMX0820221029002","imsi":"232031723329318","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0},{"id":"c6811af2822eda19","iccid":"89430301722233293198","eid":null,"sn":"TMX0820221029003","uploadedSn":"TMX0820221029003","imsi":"232031723329319","localSimStatus":"ACTIVATED","description":null,"createTime":"2022-08-31T00:01:23Z","updateTime":"2022-12-16T04:42:43Z","provider":{"id":"536bd5c4d3e18d11","name":"Simplex"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":null,"name":null},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0}]}}</t>
+        </is>
+      </c>
+      <c r="H9" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I9" s="8" t="n"/>
+      <c r="J9" s="15" t="n"/>
+    </row>
+    <row customHeight="1" ht="231" r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>查询SIM Card List--根据Group查询</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>/console/simCard/page</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>{
+ "companyId": "{company_id}",
+ "simCardGroupId": "{sim_group_id}"
+}</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>get</t>
+        </is>
+      </c>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>{
+"code":0,
+"message":"success"
+}</t>
+        </is>
+      </c>
+      <c r="G10" s="1" t="inlineStr">
+        <is>
+          <t>{"code":0,"message":"success","data":{"total":1,"pages":1,"pageSize":10,"pageNum":1,"list":[{"id":"b1fb11141bda5c33","iccid":"8935711220000105110","eid":null,"sn":null,"uploadedSn":null,"imsi":"222013095528230","localSimStatus":"ACTIVATED","description":null,"createTime":"2021-07-08T17:00:55Z","updateTime":"2022-12-30T08:27:11Z","provider":{"id":"419bd5c4d3e18d09","name":"FloLive"},"company":{"id":"788136251742011392","name":"Robot","type":0},"simCardGroup":{"id":"c37fad61fed87eac","name":"AutoGR"},"dataUsage":{"lastDay":0,"lastCycle":0,"dateToCycle":0},"dateToCycleStartDate":"2022-11-10","dateToCycleEndDate":"2022-12-28","dateToCycleDataUsage":0}]}}</t>
+        </is>
+      </c>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I10" s="8" t="n"/>
+      <c r="J10" s="15" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:C2"/>
@@ -1014,9 +1394,9 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="1"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection activeCell="D5" pane="bottomLeft" sqref="D5"/>
+      <selection activeCell="A6" pane="bottomLeft" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1031,8 +1411,8 @@
     <col customWidth="1" max="8" min="8" style="10" width="18.75"/>
     <col customWidth="1" max="9" min="9" style="3" width="19.875"/>
     <col customWidth="1" max="10" min="10" style="10" width="9"/>
-    <col customWidth="1" max="82" min="11" style="3" width="9"/>
-    <col customWidth="1" max="16384" min="83" style="3" width="9"/>
+    <col customWidth="1" max="86" min="11" style="3" width="9"/>
+    <col customWidth="1" max="16384" min="87" style="3" width="9"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="22.5" r="1">
@@ -1167,7 +1547,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":{"id":"d30b855ec56f26a9","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-13T07:19:41Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:41Z"}}</t>
+          <t>{"code":0,"message":"success","data":{"id":"33291fe90b915e29","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-15T09:00:24Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:24Z"}}</t>
         </is>
       </c>
       <c r="H3" s="7" t="inlineStr">
@@ -1216,7 +1596,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>{"code":10001,"message":"request body check error[name:taskName is not allowed to be empty,name:Group name is illegal]","data":null}</t>
+          <t>{"code":10001,"message":"request body check error[name:Group name is illegal,name:taskName is not allowed to be empty]","data":null}</t>
         </is>
       </c>
       <c r="H4" s="9" t="inlineStr">
@@ -1261,7 +1641,7 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":{"id":"53150c02a6d98d03","name":"TestGroup2","description":"","creator":"788135736837423104","createTime":"2022-12-13T07:19:42Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:42Z"}}</t>
+          <t>{"code":0,"message":"success","data":{"id":"219f5d0b8e74b4fd","name":"TestGroup2","description":"","creator":"788135736837423104","createTime":"2022-12-15T09:00:24Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:24Z"}}</t>
         </is>
       </c>
       <c r="H5" s="9" t="inlineStr">
@@ -1307,7 +1687,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":[{"id":"d30b855ec56f26a9","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-13T07:19:41Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:41Z"}]}</t>
+          <t>{"code":0,"message":"success","data":[{"id":"33291fe90b915e29","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-15T09:00:24Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:24Z"}]}</t>
         </is>
       </c>
       <c r="H6" s="9" t="inlineStr">
@@ -1355,8 +1735,8 @@
     <col customWidth="1" max="8" min="8" style="10" width="18.75"/>
     <col customWidth="1" max="9" min="9" style="3" width="19.875"/>
     <col customWidth="1" max="10" min="10" style="10" width="9"/>
-    <col customWidth="1" max="82" min="11" style="3" width="9"/>
-    <col customWidth="1" max="16384" min="83" style="3" width="9"/>
+    <col customWidth="1" max="86" min="11" style="3" width="9"/>
+    <col customWidth="1" max="16384" min="87" style="3" width="9"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="22.5" r="1">
@@ -1445,7 +1825,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":{"id":"89f0da0801dc37d2","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-13T07:19:42Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:42Z"}}</t>
+          <t>{"code":0,"message":"success","data":{"id":"6ba3e656176167ae","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-15T09:00:25Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:25Z"}}</t>
         </is>
       </c>
       <c r="H2" s="7" t="inlineStr">
@@ -1496,7 +1876,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":{"id":"89f0da0801dc37d2","name":"test","description":"123456","creator":"788135736837423104","createTime":"2022-12-13T07:19:42Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:43Z"}}</t>
+          <t>{"code":0,"message":"success","data":{"id":"6ba3e656176167ae","name":"test","description":"123456","creator":"788135736837423104","createTime":"2022-12-15T09:00:25Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:25Z"}}</t>
         </is>
       </c>
       <c r="H3" s="9" t="inlineStr">
@@ -1547,7 +1927,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":{"id":"89f0da0801dc37d2","name":"test","description":"这是修改后的描述","creator":"788135736837423104","createTime":"2022-12-13T07:19:42Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:43Z"}}</t>
+          <t>{"code":0,"message":"success","data":{"id":"6ba3e656176167ae","name":"test","description":"这是修改后的描述","creator":"788135736837423104","createTime":"2022-12-15T09:00:25Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:25Z"}}</t>
         </is>
       </c>
       <c r="H4" s="9" t="inlineStr">
@@ -1592,7 +1972,7 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":"89f0da0801dc37d2"}</t>
+          <t>{"code":0,"message":"success","data":"6ba3e656176167ae"}</t>
         </is>
       </c>
       <c r="H5" s="9" t="inlineStr">
@@ -1618,10 +1998,10 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+    <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="1"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection activeCell="F3" pane="bottomLeft" sqref="F3"/>
+      <selection activeCell="D4" pane="bottomLeft" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1636,8 +2016,8 @@
     <col customWidth="1" max="8" min="8" style="10" width="18.75"/>
     <col customWidth="1" max="9" min="9" style="3" width="19.875"/>
     <col customWidth="1" max="10" min="10" style="10" width="9"/>
-    <col customWidth="1" max="82" min="11" style="3" width="9"/>
-    <col customWidth="1" max="16384" min="83" style="3" width="9"/>
+    <col customWidth="1" max="86" min="11" style="3" width="9"/>
+    <col customWidth="1" max="16384" min="87" style="3" width="9"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="22.5" r="1">
@@ -1726,7 +2106,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>{"code":0,"message":"success","data":{"id":"19d735f16547a621","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-13T07:19:44Z","updator":"788135736837423104","updateTime":"2022-12-13T07:19:44Z"}}</t>
+          <t>{"code":0,"message":"success","data":{"id":"147ba87636fc30f8","name":"AutoGR","description":"456","creator":"788135736837423104","createTime":"2022-12-15T09:00:26Z","updator":"788135736837423104","updateTime":"2022-12-15T09:00:26Z"}}</t>
         </is>
       </c>
       <c r="H2" s="7" t="inlineStr">

</xml_diff>